<commit_message>
Se modificó la tabla comparativa y se agrego un segundo sensor de temperatura con sus repectivas caracteristicas
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029BBB92-F00F-4194-9D5F-DB71AFA420CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96316E8-B1E1-45DD-991B-F1537CADC3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="0" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="1800" yWindow="75" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -128,6 +128,47 @@
   <si>
     <t>4 min</t>
   </si>
+  <si>
+    <t>SENSOR DE TEMPERATURA TMP36</t>
+  </si>
+  <si>
+    <t>desde -50°C y 125°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análogo </t>
+  </si>
+  <si>
+    <t>2.7V - 5.5V</t>
+  </si>
+  <si>
+    <t>Medir la temperatura de los sistemas de control ambiental, protección térmica, control de procesos industriales, alarmas contra incendios, monitores de sistemas de potencia y gestión térmica de la CPU.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µA</t>
+    </r>
+  </si>
+  <si>
+    <t>10mV/°C</t>
+  </si>
+  <si>
+    <t>2°C</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/-/es/TMP36-Sensor-de-temperatura/dp/B00JYQAIBM</t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +205,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -207,11 +254,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -225,6 +269,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -254,8 +304,8 @@
       <xdr:rowOff>476250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -297,6 +347,135 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121DDA9B-C98E-494A-804F-A5DB03AD2408}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5934075" y="1428750"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1447800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E72DBA-9F61-43FC-9151-471E02035D57}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6010275" y="3543300"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -320,10 +499,10 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="CuadroTexto 1">
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121DDA9B-C98E-494A-804F-A5DB03AD2408}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E72DBA-9F61-43FC-9151-471E02035D57}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -331,7 +510,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5934075" y="1428750"/>
+              <a:off x="6010275" y="3543300"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -359,6 +538,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="es-CO" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -713,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
   <dimension ref="B2:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,140 +905,168 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="2:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+    <row r="5" spans="2:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="5">
+        <v>5900</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se modificó el tiempo de respuesta del sensor 2.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96316E8-B1E1-45DD-991B-F1537CADC3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0B1AD-553A-4FD5-AD9C-C93C57617E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="75" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Nombre</t>
   </si>
@@ -169,6 +169,9 @@
   <si>
     <t>https://www.amazon.com/-/es/TMP36-Sensor-de-temperatura/dp/B00JYQAIBM</t>
   </si>
+  <si>
+    <t>8 min</t>
+  </si>
 </sst>
 </file>
 
@@ -177,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +211,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -271,12 +282,13 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +444,8 @@
       <xdr:rowOff>1447800</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -496,7 +508,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -891,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
-  <dimension ref="B2:O6"/>
+  <dimension ref="B2:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,23 +916,23 @@
     <col min="15" max="15" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -964,7 +976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1008,15 +1020,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="240" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:16" ht="240" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>30</v>
@@ -1051,8 +1063,9 @@
       <c r="O5" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>

</xml_diff>

<commit_message>
Se agregó la columna de longitud, altura y ancho; también se agrego el dato para los tres sensores de temperatura y se agrego un tercer sensor con sus respectivas características.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0B1AD-553A-4FD5-AD9C-C93C57617E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E799A7-5E08-4B5F-BFE7-1E274A365436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="11040" yWindow="780" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -172,15 +172,64 @@
   <si>
     <t>8 min</t>
   </si>
+  <si>
+    <t>Sensor temperatura TC74</t>
+  </si>
+  <si>
+    <t>8 segundos</t>
+  </si>
+  <si>
+    <t>desde -40°C a 125°C</t>
+  </si>
+  <si>
+    <t>8 bits</t>
+  </si>
+  <si>
+    <t>https://export.rsdelivers.com/es/product/microchip/tc74a2-50vat/sensor-de-temperatura-digital-tc74a2-50vat-8-bits/1370764#____</t>
+  </si>
+  <si>
+    <t>convertir la temperatura dentro del propio sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.27 </t>
+  </si>
+  <si>
+    <t>Longitud (mm)</t>
+  </si>
+  <si>
+    <t>Altura (mm)</t>
+  </si>
+  <si>
+    <t>Ancho (mm)</t>
+  </si>
+  <si>
+    <t>15.17</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>5.33</t>
+  </si>
+  <si>
+    <t>4.19</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +271,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="3">
@@ -265,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -285,10 +339,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,7 +373,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>476250</xdr:rowOff>
@@ -438,14 +501,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129198</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1447800</xdr:rowOff>
+      <xdr:rowOff>1508858</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -459,7 +522,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6010275" y="3543300"/>
+              <a:off x="6027371" y="3621454"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -508,7 +571,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -522,7 +585,136 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6010275" y="3543300"/>
+              <a:off x="6027371" y="3621454"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171694</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>122604</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B233364-F93F-4A9C-872C-20AA1271AFF1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6069867" y="5446835"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B233364-F93F-4A9C-872C-20AA1271AFF1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6069867" y="5446835"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -903,36 +1095,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
-  <dimension ref="B2:P6"/>
+  <dimension ref="B2:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+    <row r="2" spans="2:19">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="45">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -940,87 +1135,105 @@
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="90">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4">
+      <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="252.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1028,62 +1241,108 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="5">
+      <c r="Q5" s="5">
         <v>5900</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="8"/>
+      <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+    <row r="6" spans="2:19" ht="97.5" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>61.05</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó un cuarto sensor de temperatura a la tabla.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E799A7-5E08-4B5F-BFE7-1E274A365436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABEEC70-8E9F-4998-9166-C3B094B21A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="780" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="5790" yWindow="0" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -220,16 +220,41 @@
   <si>
     <t>Digital</t>
   </si>
+  <si>
+    <t>SENSORES DE TEMPERATURA</t>
+  </si>
+  <si>
+    <t>Sensor temperatura DHT11</t>
+  </si>
+  <si>
+    <t>VCC, DATA, NC, GND</t>
+  </si>
+  <si>
+    <t>conversión a grados centígrados.</t>
+  </si>
+  <si>
+    <t>0.5 segundos</t>
+  </si>
+  <si>
+    <t>3V - 5V dc</t>
+  </si>
+  <si>
+    <t>desde 0°C a 50°C</t>
+  </si>
+  <si>
+    <t>https://naylampmechatronics.com/sensores-temperatura-y-humedad/57-sensor-de-temperatura-y-humedad-relativa-dht11.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +302,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri "/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -292,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -315,11 +346,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -340,16 +382,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -376,11 +427,11 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>476250</xdr:rowOff>
+      <xdr:rowOff>342564</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -394,7 +445,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5934075" y="1428750"/>
+              <a:off x="12711864" y="1478880"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -443,7 +494,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -457,7 +508,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5934075" y="1428750"/>
+              <a:off x="12711864" y="1478880"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -485,6 +536,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="es-CO" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -502,9 +554,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>129198</xdr:colOff>
+      <xdr:colOff>145908</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1508858</xdr:rowOff>
+      <xdr:rowOff>690043</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -522,7 +574,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6027371" y="3621454"/>
+              <a:off x="12829197" y="2661885"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -585,7 +637,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6027371" y="3621454"/>
+              <a:off x="12829197" y="2661885"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -631,9 +683,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>171694</xdr:colOff>
+      <xdr:colOff>287951</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>122604</xdr:rowOff>
+      <xdr:rowOff>513152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -651,7 +703,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6069867" y="5446835"/>
+              <a:off x="13595737" y="4064616"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -714,7 +766,136 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6069867" y="5446835"/>
+              <a:off x="13595737" y="4064616"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>287952</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>349867</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6F2906-2450-4AF8-ACC6-807144558978}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13595738" y="5139581"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6F2906-2450-4AF8-ACC6-807144558978}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13595738" y="5139581"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1095,39 +1276,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
-  <dimension ref="B2:S6"/>
+  <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="31" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" customWidth="1"/>
+    <col min="18" max="18" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="B2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
     </row>
-    <row r="3" spans="2:19" ht="45">
+    <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1180,14 +1371,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="90">
+    <row r="4" spans="2:19" ht="66" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1233,7 +1424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="252.75" customHeight="1">
+    <row r="5" spans="2:19" ht="122.25" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1291,7 +1482,7 @@
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1333,12 +1524,68 @@
       <c r="P6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="11">
         <v>61.05</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="7" spans="2:19" ht="74.25" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>10</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19">
+      <c r="P8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se agregó un quinto sensor de temperatura y se agregaron datos faltantes de los sensores anteriores a la tabla.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABEEC70-8E9F-4998-9166-C3B094B21A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B598A1-500A-4EDF-B6CC-CED4A5B31D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="0" windowWidth="14700" windowHeight="11520" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="19335" windowHeight="11760" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Nombre</t>
   </si>
@@ -244,6 +244,67 @@
   <si>
     <t>https://naylampmechatronics.com/sensores-temperatura-y-humedad/57-sensor-de-temperatura-y-humedad-relativa-dht11.html</t>
   </si>
+  <si>
+    <t>Sensor temperatura  DHT22</t>
+  </si>
+  <si>
+    <t>3.3 V a 6V</t>
+  </si>
+  <si>
+    <t>16 bits</t>
+  </si>
+  <si>
+    <t>0.5°C</t>
+  </si>
+  <si>
+    <t>desde -40°C a 80°C</t>
+  </si>
+  <si>
+    <t>2 segundos</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µA</t>
+    </r>
+  </si>
+  <si>
+    <t>necesita medir los niveles de temperatura y humedad de ciertos ambientes</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>https://naylampmechatronics.com/sensores-temperatura-y-humedad/58-sensor-de-temperatura-y-humedad-relativa-dht22-am2302.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µA</t>
+    </r>
+  </si>
+  <si>
+    <t>NC, SDA, GND, VDD, SCLIK</t>
+  </si>
+  <si>
+    <t>Vin, Vout, GND</t>
+  </si>
 </sst>
 </file>
 
@@ -251,8 +312,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -323,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -344,17 +405,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -388,19 +438,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -430,8 +480,8 @@
       <xdr:rowOff>342564</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -494,7 +544,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -559,8 +609,8 @@
       <xdr:rowOff>690043</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -623,7 +673,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -688,8 +738,8 @@
       <xdr:rowOff>513152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -752,7 +802,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -812,7 +862,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>287952</xdr:colOff>
+      <xdr:colOff>328774</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>349867</xdr:rowOff>
     </xdr:from>
@@ -832,7 +882,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13595738" y="5139581"/>
+              <a:off x="13636560" y="5139581"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -895,7 +945,136 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13595738" y="5139581"/>
+              <a:off x="13636560" y="5139581"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317888</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>393411</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13625674" y="6122018"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13625674" y="6122018"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1278,13 +1457,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
   <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
     <col min="3" max="3" width="69.5703125" customWidth="1"/>
     <col min="4" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
@@ -1298,25 +1478,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="3" t="s">
@@ -1447,7 +1627,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>34</v>
@@ -1455,11 +1635,11 @@
       <c r="K5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>35</v>
+      <c r="L5" s="1">
+        <v>3</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
@@ -1501,19 +1681,19 @@
         <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>35</v>
+      <c r="K6" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="L6" s="1">
         <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>53</v>
@@ -1524,7 +1704,7 @@
       <c r="P6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6" s="10">
         <v>61.05</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1535,7 +1715,7 @@
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="1">
@@ -1554,13 +1734,13 @@
         <v>59</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>35</v>
+      <c r="K7" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="L7" s="1">
         <v>4</v>
@@ -1577,15 +1757,65 @@
       <c r="P7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="12">
         <v>10</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:19">
-      <c r="P8" s="13"/>
+    <row r="8" spans="2:19" ht="75" customHeight="1">
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="4">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se agregó una nueva hoja con sensores para automatizaciones de temperatura; también se modifico la tabla de acuerdo a las cacracterísticas y se agrega el primer sensor.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B598A1-500A-4EDF-B6CC-CED4A5B31D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F7E92-DA70-4634-A633-9C360E0DEFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="19335" windowHeight="11760" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="5790" yWindow="0" windowWidth="14700" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensores temperatura automat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
   <si>
     <t>Nombre</t>
   </si>
@@ -304,6 +305,89 @@
   </si>
   <si>
     <t>Vin, Vout, GND</t>
+  </si>
+  <si>
+    <t>SENSORES DE TEMPERATURA AUTOMATIZACIONES</t>
+  </si>
+  <si>
+    <t>Sensor SHT15</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Esta es una simple breakout board para el sensor de humedad SHT15 de Sensirion. El sensor digital de humedad y temperatura está completamente calibrado, ofrece una alta precisión y una excelente estabilidad a bajo costo. La tecnología CMOSens integra 2 sensores y circuitos de lectura en un sólo chip.Estos sensores son muy sensibles y sencillos de usar. La placa viene ensamblada y probada con el SHT15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - 100% </t>
+  </si>
+  <si>
+    <t>Rango de medición (RH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2% RH</t>
+  </si>
+  <si>
+    <t>Precisión de RH absoluta (10 … 90% RH)</t>
+  </si>
+  <si>
+    <t>Repetición de RH</t>
+  </si>
+  <si>
+    <t>0.1 % RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo de respuesta </t>
+  </si>
+  <si>
+    <t>&lt;4 segundos</t>
+  </si>
+  <si>
+    <t>14 bit</t>
+  </si>
+  <si>
+    <t>desde -40°C hasta 123.8°C</t>
+  </si>
+  <si>
+    <t>Rango temperatura</t>
+  </si>
+  <si>
+    <t>0.3 °C a 25°C</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µW</t>
+    </r>
+  </si>
+  <si>
+    <t>http://www.controlcomp.com/inicio/31-humidity_and_temperature_sensor_sht15_breakout.html</t>
+  </si>
+  <si>
+    <t>2.4V - 5.5 V</t>
+  </si>
+  <si>
+    <t>Tipo de montaje</t>
+  </si>
+  <si>
+    <t>Montaje en superficie</t>
+  </si>
+  <si>
+    <t>Tipo de sensor</t>
+  </si>
+  <si>
+    <t>Humedad, temperatura</t>
+  </si>
+  <si>
+    <t>Peso (g)</t>
   </si>
 </sst>
 </file>
@@ -370,7 +454,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +464,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,9 +509,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -447,10 +534,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,6 +549,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -867,8 +962,8 @@
       <xdr:rowOff>349867</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4">
@@ -883,6 +978,656 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="13636560" y="5139581"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6F2906-2450-4AF8-ACC6-807144558978}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13636560" y="5139581"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317888</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>393411</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13625674" y="6122018"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13625674" y="6122018"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>799764</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3A09EC-360B-49E3-AD17-5B2C811673C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7839075" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3A09EC-360B-49E3-AD17-5B2C811673C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7839075" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>145908</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>690043</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13909533" y="2680768"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13909533" y="2680768"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>287951</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>513152</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14051576" y="4056452"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14051576" y="4056452"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>328774</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>349867</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14092399" y="5131417"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -937,7 +1682,7 @@
             <xdr:cNvPr id="5" name="CuadroTexto 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6F2906-2450-4AF8-ACC6-807144558978}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -945,7 +1690,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13636560" y="5139581"/>
+              <a:off x="14092399" y="5131417"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1003,7 +1748,7 @@
             <xdr:cNvPr id="6" name="CuadroTexto 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1011,7 +1756,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13625674" y="6122018"/>
+              <a:off x="14081513" y="6117936"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1066,7 +1811,7 @@
             <xdr:cNvPr id="6" name="CuadroTexto 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F1AA09-4FF7-4078-82A9-B79C25E024F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1074,7 +1819,265 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13625674" y="6122018"/>
+              <a:off x="14081513" y="6117936"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>799764</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9077325" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9077325" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>771525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13630275" y="1914525"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13630275" y="1914525"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1457,8 +2460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72CEDC0-C820-4510-AAD8-AF0AAF2EC465}">
   <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1499,55 +2502,55 @@
       <c r="R2" s="13"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1558,7 +2561,7 @@
       <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1570,19 +2573,19 @@
       <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>3</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -1597,7 +2600,7 @@
       <c r="P4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1605,7 +2608,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" ht="122.25" customHeight="1">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1632,7 +2635,7 @@
       <c r="J5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L5" s="1">
@@ -1650,19 +2653,19 @@
       <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="4">
         <v>5900</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="7"/>
+      <c r="S5" s="6"/>
     </row>
     <row r="6" spans="2:19" ht="97.5" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1686,7 +2689,7 @@
       <c r="J6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="L6" s="1">
@@ -1704,7 +2707,7 @@
       <c r="P6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="9">
         <v>61.05</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1715,7 +2718,7 @@
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="1">
@@ -1739,7 +2742,7 @@
       <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="3" t="s">
         <v>68</v>
       </c>
       <c r="L7" s="1">
@@ -1757,7 +2760,7 @@
       <c r="P7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="11">
         <v>10</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -1771,46 +2774,46 @@
       <c r="C8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>20</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>15</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>8</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>4</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="Q8" s="11">
         <v>20</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -1825,4 +2828,239 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC1976-CDDE-4A3F-AE37-3B9B7D1D1CB0}">
+  <dimension ref="B2:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18">
+      <c r="B2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="2:18" ht="60" customHeight="1">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="135" customHeight="1">
+      <c r="B4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" s="1">
+        <v>998</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>80</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="5"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
En la hoja de excel nueva se agrega un segundo sensor que no se encuentra facilmente en el mercado.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F7E92-DA70-4634-A633-9C360E0DEFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DDE6B9-09F8-4103-80BE-48AC79DD718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5790" yWindow="0" windowWidth="14700" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
   <si>
     <t>Nombre</t>
   </si>
@@ -388,6 +388,50 @@
   </si>
   <si>
     <t>Peso (g)</t>
+  </si>
+  <si>
+    <t>Sensor Thermocouple Type-k</t>
+  </si>
+  <si>
+    <t>desde -50°C hasta 1200°C</t>
+  </si>
+  <si>
+    <t>Humedad</t>
+  </si>
+  <si>
+    <t>0 - 1100</t>
+  </si>
+  <si>
+    <t>2 - 3,8 Vdc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µW - 22.6 µA</t>
+    </r>
+  </si>
+  <si>
+    <t>No disponible</t>
+  </si>
+  <si>
+    <t>1.5 °C</t>
+  </si>
+  <si>
+    <t>10 segundos</t>
+  </si>
+  <si>
+    <t>Este tipo de sensores no tiene nada de electrónica. Consiste en un par de cables de metal soldados. Se puede medir el voltaje que circula por estos dos cables juntos cuando sube la temperatura, debido a la naturaleza de este tipo de metales.</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/-/es/Thermocouple-PK-1-temperatura-aislamiento-plástico/dp/B0083T16X0</t>
   </si>
 </sst>
 </file>
@@ -537,11 +581,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,8 +1269,8 @@
       <xdr:rowOff>799764</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1241,6 +1285,909 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7839075" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3A09EC-360B-49E3-AD17-5B2C811673C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7839075" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>145908</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>690043</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13909533" y="2680768"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13909533" y="2680768"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>287951</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>513152</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14051576" y="4056452"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14051576" y="4056452"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>328774</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>349867</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14092399" y="5131417"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="CuadroTexto 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14092399" y="5131417"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317888</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>393411</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14081513" y="6117936"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="CuadroTexto 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14081513" y="6117936"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>799764</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9077325" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9077325" y="1942764"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>771525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13630275" y="1914525"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13630275" y="1914525"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="CuadroTexto 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777B6A88-CD55-4A1D-B73F-AE7EFB3C1B01}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13877925" y="3152775"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1292,10 +2239,10 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="CuadroTexto 1">
+            <xdr:cNvPr id="9" name="CuadroTexto 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3A09EC-360B-49E3-AD17-5B2C811673C8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777B6A88-CD55-4A1D-B73F-AE7EFB3C1B01}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1303,781 +2250,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7839075" y="1942764"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145908</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>690043</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="CuadroTexto 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13909533" y="2680768"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="CuadroTexto 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13909533" y="2680768"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>287951</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>513152</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="CuadroTexto 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14051576" y="4056452"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="CuadroTexto 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14051576" y="4056452"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>328774</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>349867</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="CuadroTexto 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14092399" y="5131417"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="CuadroTexto 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14092399" y="5131417"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>317888</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>393411</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="CuadroTexto 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14081513" y="6117936"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="CuadroTexto 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14081513" y="6117936"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>799764</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="CuadroTexto 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9077325" y="1942764"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="CuadroTexto 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9077325" y="1942764"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>771525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="CuadroTexto 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13630275" y="1914525"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="CuadroTexto 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13630275" y="1914525"/>
+              <a:off x="13877925" y="3152775"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2481,76 +2654,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2834,13 +3007,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC1976-CDDE-4A3F-AE37-3B9B7D1D1CB0}">
   <dimension ref="B2:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
@@ -2848,82 +3021,83 @@
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" customWidth="1"/>
     <col min="18" max="18" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
     <row r="3" spans="2:18" ht="60" customHeight="1">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2980,24 +3154,58 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:18">
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="1"/>
+    <row r="5" spans="2:18" ht="60">
+      <c r="B5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" s="1">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="1"/>
@@ -3061,6 +3269,7 @@
     <mergeCell ref="B2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega un otra categoria de sensores en la hoja 2 y un sensor con su respctiva caracteristicas.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DDE6B9-09F8-4103-80BE-48AC79DD718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52849CC-7862-413B-AAD1-BC3610413FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="0" windowWidth="14700" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="11085" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="144">
   <si>
     <t>Nombre</t>
   </si>
@@ -432,6 +432,108 @@
   </si>
   <si>
     <t>https://www.amazon.com/-/es/Thermocouple-PK-1-temperatura-aislamiento-plástico/dp/B0083T16X0</t>
+  </si>
+  <si>
+    <t>SENSORES DE TEMPERATURA CON CARACTEERÍSTICAS ESPECIALES</t>
+  </si>
+  <si>
+    <t>Sensor de temperatura MLX90614ESF</t>
+  </si>
+  <si>
+    <t>Conexión</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>3.3V  +/- 5 V dc</t>
+  </si>
+  <si>
+    <t>0V tierra</t>
+  </si>
+  <si>
+    <t>I2C clock</t>
+  </si>
+  <si>
+    <t>I2C data</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>GY- 906</t>
+  </si>
+  <si>
+    <t>Voltaje de operación</t>
+  </si>
+  <si>
+    <t>3.3 V - 5V DC</t>
+  </si>
+  <si>
+    <t>Rango de temperatura ambiente de trabajo</t>
+  </si>
+  <si>
+    <t>desde -40°C hasta 170°C</t>
+  </si>
+  <si>
+    <t>Rango de temperatura de objeto</t>
+  </si>
+  <si>
+    <t>desde -70°C hasta 380°C</t>
+  </si>
+  <si>
+    <t>ADC interno</t>
+  </si>
+  <si>
+    <t>17 bits</t>
+  </si>
+  <si>
+    <t>Regulador de voltaje en placa</t>
+  </si>
+  <si>
+    <t>3.3 V</t>
+  </si>
+  <si>
+    <t>16*11*6</t>
+  </si>
+  <si>
+    <t>Dimensiones (mm)</t>
+  </si>
+  <si>
+    <t>2.80</t>
+  </si>
+  <si>
+    <t>https://naylampmechatronics.com/sensores-temperatura-y-humedad/330-sensor-de-temperatura-mlx90614.html</t>
+  </si>
+  <si>
+    <t>Adaptación simple</t>
+  </si>
+  <si>
+    <t>8V - 16V</t>
+  </si>
+  <si>
+    <t>Salida</t>
+  </si>
+  <si>
+    <t>PWM adaptable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacto </t>
+  </si>
+  <si>
+    <t>Modo</t>
+  </si>
+  <si>
+    <t>Ahorro de energía</t>
   </si>
 </sst>
 </file>
@@ -498,7 +600,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,8 +619,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -541,11 +649,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -586,6 +768,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,6 +846,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FF66FFCC"/>
     </mruColors>
   </colors>
@@ -1263,14 +1515,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411431</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>799764</xdr:rowOff>
+      <xdr:rowOff>1158498</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1284,7 +1536,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7839075" y="1942764"/>
+              <a:off x="5619256" y="2296550"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1333,7 +1585,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1347,7 +1599,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7839075" y="1942764"/>
+              <a:off x="5619256" y="2296550"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1392,20 +1644,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145908</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>690043</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>359845</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1170871</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="CuadroTexto 2">
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1413,7 +1665,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13909533" y="2680768"/>
+              <a:off x="7002605" y="2308923"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1462,13 +1714,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="CuadroTexto 2">
+            <xdr:cNvPr id="7" name="CuadroTexto 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5176FD-D502-4475-BF04-446C0EC25BDF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1476,7 +1728,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13909533" y="2680768"/>
+              <a:off x="7002605" y="2308923"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1521,20 +1773,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>287951</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>513152</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1167369</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="CuadroTexto 3">
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1542,7 +1794,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14051576" y="4056452"/>
+              <a:off x="11779332" y="2305421"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1591,13 +1843,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="CuadroTexto 3">
+            <xdr:cNvPr id="8" name="CuadroTexto 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12108078-FF06-401B-AAF3-F5511BB6A7B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,7 +1857,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14051576" y="4056452"/>
+              <a:off x="11779332" y="2305421"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1650,526 +1902,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>328774</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>349867</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="CuadroTexto 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14092399" y="5131417"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="CuadroTexto 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E645C3D-61CD-4DFA-A61B-587566D3C237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14092399" y="5131417"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>317888</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>393411</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="CuadroTexto 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14081513" y="6117936"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="CuadroTexto 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C685D4D-3968-40F0-9224-A3CA29586CBC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14081513" y="6117936"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>799764</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="CuadroTexto 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9077325" y="1942764"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="CuadroTexto 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1DBF86-7015-4044-9D95-AE93758729BF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9077325" y="1942764"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>771525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="CuadroTexto 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13630275" y="1914525"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="es-CO" sz="1100">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>±</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="CuadroTexto 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7812DF-B6D5-4569-B469-0FE3296297D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13630275" y="1914525"/>
-              <a:ext cx="137282" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="es-CO" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>±</a:t>
-              </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>310491</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>790078</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2187,7 +1923,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13877925" y="3152775"/>
+              <a:off x="11975523" y="4439266"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2250,7 +1986,136 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13877925" y="3152775"/>
+              <a:off x="11975523" y="4439266"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>363928</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>460044</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137282" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="CuadroTexto 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A0B8D7-6855-4304-804B-AE5CF8A04143}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9938409" y="5606018"/>
+              <a:ext cx="137282" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-CO" sz="1100">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>±</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="CuadroTexto 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A0B8D7-6855-4304-804B-AE5CF8A04143}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9938409" y="5606018"/>
               <a:ext cx="137282" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3005,29 +2870,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC1976-CDDE-4A3F-AE37-3B9B7D1D1CB0}">
-  <dimension ref="B2:R8"/>
+  <dimension ref="B2:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="41" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18">
+    <row r="2" spans="2:19">
       <c r="B2" s="14" t="s">
         <v>75</v>
       </c>
@@ -3047,226 +2913,422 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
     </row>
-    <row r="3" spans="2:18" ht="60" customHeight="1">
+    <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="J3" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="135" customHeight="1">
+    <row r="4" spans="2:19" ht="197.25" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>998</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="R4" s="11">
         <v>80</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="60">
+    <row r="5" spans="2:19" ht="139.5" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>24</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="2:18">
-      <c r="B6" s="1"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="1"/>
+    <row r="6" spans="2:19">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="2:18">
-      <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="1"/>
+    <row r="7" spans="2:19">
+      <c r="B7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
     </row>
-    <row r="8" spans="2:18">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="1"/>
+    <row r="8" spans="2:19" ht="69" customHeight="1">
+      <c r="B8" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="O8" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q8" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="45" customHeight="1">
+      <c r="B9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="R9" s="34">
+        <v>90</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="B10" s="24"/>
+      <c r="C10" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="24"/>
+    </row>
+    <row r="11" spans="2:19">
+      <c r="B11" s="24"/>
+      <c r="C11" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="24"/>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="25"/>
+      <c r="C12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:R2"/>
+  <mergeCells count="23">
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega un nuevo sensor con su respctiva caracteristicas.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52849CC-7862-413B-AAD1-BC3610413FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E37ADE3-C81A-4228-BCB8-BD135B48E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11085" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="171">
   <si>
     <t>Nombre</t>
   </si>
@@ -535,17 +535,99 @@
   <si>
     <t>Ahorro de energía</t>
   </si>
+  <si>
+    <t>Sensor de temperatura D6T MEMS</t>
+  </si>
+  <si>
+    <t>Tipo de salida</t>
+  </si>
+  <si>
+    <t>Exactitud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  +/-1. 5 C</t>
+  </si>
+  <si>
+    <t>4.5 V - 5.5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intefaz </t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>desde -40°C hasta 80°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rango de temperatura </t>
+  </si>
+  <si>
+    <t>Estilo de  montaje</t>
+  </si>
+  <si>
+    <t>PCB Mount</t>
+  </si>
+  <si>
+    <t>Empaquetado</t>
+  </si>
+  <si>
+    <t>Tray</t>
+  </si>
+  <si>
+    <t>Corriente de suministro operativo</t>
+  </si>
+  <si>
+    <t>3.5 mA</t>
+  </si>
+  <si>
+    <t>Serie</t>
+  </si>
+  <si>
+    <t>D6T</t>
+  </si>
+  <si>
+    <t>653-D6T-1A-02</t>
+  </si>
+  <si>
+    <t>Mouse N°</t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Temperature Sensors</t>
+  </si>
+  <si>
+    <t>Detención de puntos calientes</t>
+  </si>
+  <si>
+    <t>Inmunidad al ruido</t>
+  </si>
+  <si>
+    <t>Por medio de salida digital</t>
+  </si>
+  <si>
+    <t>https://es.farnell.com/omron/d6t-44l-06/sensor-thermal-mems-4x4/dp/2218000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +680,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="5">
@@ -727,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -766,9 +857,57 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,52 +929,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1521,8 +1642,8 @@
       <xdr:rowOff>1158498</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1585,7 +1706,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1650,8 +1771,8 @@
       <xdr:rowOff>1170871</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -1714,7 +1835,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -1779,8 +1900,8 @@
       <xdr:rowOff>1167369</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -1843,7 +1964,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -1908,8 +2029,8 @@
       <xdr:rowOff>790078</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -1972,7 +2093,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -2037,8 +2158,8 @@
       <xdr:rowOff>460044</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137282" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 11">
@@ -2101,7 +2222,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 11">
@@ -2519,25 +2640,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="13" t="s">
@@ -2870,10 +2991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC1976-CDDE-4A3F-AE37-3B9B7D1D1CB0}">
-  <dimension ref="B2:S13"/>
+  <dimension ref="B2:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2886,43 +3007,47 @@
     <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="23.5703125" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" customWidth="1"/>
     <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
     <col min="19" max="19" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
     </row>
     <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -2973,10 +3098,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3027,10 +3152,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3078,98 +3203,98 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="33"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
     </row>
     <row r="8" spans="2:19" ht="69" customHeight="1">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="N8" s="30" t="s">
+      <c r="N8" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="O8" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="P8" s="30" t="s">
+      <c r="P8" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="Q8" s="30" t="s">
+      <c r="Q8" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="30" t="s">
+      <c r="S8" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3183,10 +3308,10 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="28" t="s">
         <v>124</v>
       </c>
       <c r="G9" s="23" t="s">
@@ -3222,7 +3347,7 @@
       <c r="Q9" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="34">
+      <c r="R9" s="20">
         <v>90</v>
       </c>
       <c r="S9" s="23" t="s">
@@ -3231,14 +3356,14 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="24"/>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
@@ -3250,19 +3375,19 @@
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
-      <c r="R10" s="35"/>
+      <c r="R10" s="21"/>
       <c r="S10" s="24"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="24"/>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -3274,19 +3399,19 @@
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
-      <c r="R11" s="35"/>
+      <c r="R11" s="21"/>
       <c r="S11" s="24"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="25"/>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3298,14 +3423,188 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
       <c r="Q12" s="25"/>
-      <c r="R12" s="36"/>
+      <c r="R12" s="22"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="2:19">
-      <c r="B13" s="37"/>
+    <row r="13" spans="2:19" ht="30">
+      <c r="B13" s="38"/>
+      <c r="C13" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="L13" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="M13" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="N13" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="O13" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="P13" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" ht="51.75" customHeight="1">
+      <c r="B14" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>3500</v>
+      </c>
+      <c r="R14" s="43">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3313,22 +3612,6 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se CREA UNA HOJA DE SENSORES DE HUMEDAD Y SE AÑADE EL PRIMER SENSOR
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E37ADE3-C81A-4228-BCB8-BD135B48E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C7D6BC-419E-4BEE-8483-FD3D85A885CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="1" activeTab="1" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="19335" windowHeight="11760" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
     <sheet name="Sensores temperatura automat" sheetId="2" r:id="rId2"/>
+    <sheet name="Sensores de humedad" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="195">
   <si>
     <t>Nombre</t>
   </si>
@@ -616,6 +617,99 @@
   <si>
     <t>https://es.farnell.com/omron/d6t-44l-06/sensor-thermal-mems-4x4/dp/2218000</t>
   </si>
+  <si>
+    <t>Sensor de humedad PCE-P18</t>
+  </si>
+  <si>
+    <t>Rango de medición</t>
+  </si>
+  <si>
+    <t>0 … 100% H.r.</t>
+  </si>
+  <si>
+    <t>(en el rango 10 .... 90 % H.r.)  +-2%                                ± 3 % (resto de rango)</t>
+  </si>
+  <si>
+    <t>Rango medición temperatura</t>
+  </si>
+  <si>
+    <t>desde -20 hasta 60°C</t>
+  </si>
+  <si>
+    <t>Corriente</t>
+  </si>
+  <si>
+    <t>4 - 20 mA</t>
+  </si>
+  <si>
+    <t>Tensión</t>
+  </si>
+  <si>
+    <t>0 - 10 V</t>
+  </si>
+  <si>
+    <t>Resistencia máxima conectable en la salida</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt;= 100 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y &lt;=1 KΩ</t>
+    </r>
+  </si>
+  <si>
+    <t>Potencia</t>
+  </si>
+  <si>
+    <t>Tiempo de precalentamiento</t>
+  </si>
+  <si>
+    <t>&lt; 1.5 W</t>
+  </si>
+  <si>
+    <t>15 minutos</t>
+  </si>
+  <si>
+    <t>Dimensiones</t>
+  </si>
+  <si>
+    <t>35 * 58* 118 mm</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>125 g</t>
+  </si>
+  <si>
+    <t>Temperatura ambiental</t>
+  </si>
+  <si>
+    <t>desde -30 hasta 85°C</t>
+  </si>
+  <si>
+    <t>https://www.pce-instruments.com/colombia/sistemas-regulacion-control/sensorica/sensor-humedad-pce-instruments-sensor-de-humedad-y-temperatura-serie-pce-p18-det_5869255.htm</t>
+  </si>
+  <si>
+    <t>SENSORES DE HUMEDAD</t>
+  </si>
 </sst>
 </file>
 
@@ -625,9 +719,9 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,8 +784,16 @@
       <sz val="11"/>
       <name val="Calibri "/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +815,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,10 +923,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -872,9 +981,84 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -884,89 +1068,28 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FF66FFCC"/>
     </mruColors>
@@ -2640,25 +2763,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="13" t="s">
@@ -2993,7 +3116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC1976-CDDE-4A3F-AE37-3B9B7D1D1CB0}">
   <dimension ref="B2:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3019,35 +3142,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3098,10 +3221,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3152,10 +3275,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3203,55 +3326,55 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="33"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="32"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
     </row>
     <row r="8" spans="2:19" ht="69" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3299,7 +3422,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="39" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3308,171 +3431,171 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="23" t="s">
+      <c r="O9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="P9" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="20">
+      <c r="R9" s="45">
         <v>90</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="S9" s="39" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="24"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="24"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="40"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="24"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="24"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="40"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="25"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="25"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="41"/>
     </row>
     <row r="13" spans="2:19" ht="30">
-      <c r="B13" s="38"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="17" t="s">
         <v>145</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="40" t="s">
+      <c r="G13" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="H13" s="40" t="s">
+      <c r="H13" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="40" t="s">
+      <c r="J13" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="L13" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="M13" s="40" t="s">
+      <c r="M13" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="N13" s="40" t="s">
+      <c r="N13" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="O13" s="40" t="s">
+      <c r="O13" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="P13" s="40" t="s">
+      <c r="P13" s="21" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="51.75" customHeight="1">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="22" t="s">
         <v>144</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3517,10 +3640,10 @@
       <c r="P14" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="Q14" s="42">
+      <c r="Q14" s="23">
         <v>3500</v>
       </c>
-      <c r="R14" s="43">
+      <c r="R14" s="24">
         <v>35.979999999999997</v>
       </c>
       <c r="S14" s="1" t="s">
@@ -3528,83 +3651,67 @@
       </c>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3612,9 +3719,212 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418314EB-8B6F-4509-AC06-8A64A9DA32C2}">
+  <dimension ref="B2:O7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="13" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="78.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15">
+      <c r="B2" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+    </row>
+    <row r="3" spans="2:15" ht="60">
+      <c r="B3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="M3" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="N3" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="87.75" customHeight="1">
+      <c r="B4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N4" s="48">
+        <v>1070286</v>
+      </c>
+      <c r="O4" s="49" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:O2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O4" r:id="rId1" xr:uid="{9EEA6375-A6E6-4F08-8DD2-33316D0A31CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega un segundo y ter sensensor e humedad (el teercero solo cuenta con el nombre)
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C7D6BC-419E-4BEE-8483-FD3D85A885CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B29E6FB-F75A-4709-AEF8-F8B776988C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="19335" windowHeight="11760" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="11085" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="221">
   <si>
     <t>Nombre</t>
   </si>
@@ -709,6 +709,84 @@
   </si>
   <si>
     <t>SENSORES DE HUMEDAD</t>
+  </si>
+  <si>
+    <t>MTH100 Sensor de humedad y temperatura</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>RH: 3%RH, T: +/- 0.3</t>
+  </si>
+  <si>
+    <t>Long Stability</t>
+  </si>
+  <si>
+    <t>T: &lt;0.04°C/year</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>t: -20 to 80°C; 0 to 50°C; -40 to 60°C;;  RH: 0 - 99.9%</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>T: 0.1°C,    RH: 0.1%RH</t>
+  </si>
+  <si>
+    <t>Load resistor</t>
+  </si>
+  <si>
+    <t>&lt; 500 ohm (4-20 mA)</t>
+  </si>
+  <si>
+    <t>Power consumption</t>
+  </si>
+  <si>
+    <t>1 VmA</t>
+  </si>
+  <si>
+    <t>Storage temperature</t>
+  </si>
+  <si>
+    <t>T: 40 to 80°C;  H: 0 -99.9%</t>
+  </si>
+  <si>
+    <t>Housing material</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>Case size</t>
+  </si>
+  <si>
+    <t>89*110*38 mm</t>
+  </si>
+  <si>
+    <t>Response time</t>
+  </si>
+  <si>
+    <t>T: 6t(63%): min = 5s,  max=30s;   H(90%): 8s</t>
+  </si>
+  <si>
+    <t>&lt;500 ohm</t>
+  </si>
+  <si>
+    <t>https://srcsl.com/catalogoPDFs/SensoresProce/SensoresHumedad/MTH500H.pdf</t>
+  </si>
+  <si>
+    <t>USD  25 - 35</t>
+  </si>
+  <si>
+    <t>MTH500H Sensor de humedad y temperatura</t>
   </si>
 </sst>
 </file>
@@ -1011,9 +1089,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1035,50 +1155,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2763,25 +2841,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="13" t="s">
@@ -3142,35 +3220,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
     </row>
     <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3221,10 +3299,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3275,10 +3353,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3326,55 +3404,55 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="32"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="46"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
     </row>
     <row r="8" spans="2:19" ht="69" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="38"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3422,7 +3500,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3431,123 +3509,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="39" t="s">
+      <c r="Q9" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="45">
+      <c r="R9" s="33">
         <v>90</v>
       </c>
-      <c r="S9" s="39" t="s">
+      <c r="S9" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="40"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="40"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="37"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="40"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="37"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="41"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="41"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="38"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -3712,6 +3790,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3719,22 +3813,6 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3746,8 +3824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418314EB-8B6F-4509-AC06-8A64A9DA32C2}">
   <dimension ref="B2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3755,73 +3833,75 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="13" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="78.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="2:15" ht="60">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="M3" s="51" t="s">
+      <c r="M3" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="N3" s="51" t="s">
+      <c r="N3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="O3" s="31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3862,47 +3942,105 @@
       <c r="M4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="29">
         <v>1070286</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="30" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+    <row r="5" spans="2:15" ht="30">
+      <c r="B5" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="2:15">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+    <row r="6" spans="2:15" ht="45">
+      <c r="B6" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="1"/>
+    <row r="7" spans="2:15" ht="45">
+      <c r="B7" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3914,7 +4052,9 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="O7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega la información del tercer sensor de humedad.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B29E6FB-F75A-4709-AEF8-F8B776988C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F695A8-7EDB-4680-A90C-3F37305BDD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="10905" yWindow="4740" windowWidth="9405" windowHeight="11520" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="227">
   <si>
     <t>Nombre</t>
   </si>
@@ -774,9 +774,6 @@
     <t>Response time</t>
   </si>
   <si>
-    <t>T: 6t(63%): min = 5s,  max=30s;   H(90%): 8s</t>
-  </si>
-  <si>
     <t>&lt;500 ohm</t>
   </si>
   <si>
@@ -787,6 +784,27 @@
   </si>
   <si>
     <t>MTH500H Sensor de humedad y temperatura</t>
+  </si>
+  <si>
+    <t>T: +/- 0.3°C;  RH: 3%RH</t>
+  </si>
+  <si>
+    <t>t: &lt;0.04°C/year; RH: &lt;0.05 RH/year</t>
+  </si>
+  <si>
+    <t>t: -20 to 80°C</t>
+  </si>
+  <si>
+    <t>15mA</t>
+  </si>
+  <si>
+    <t>T: 6t(63%): min = 2s,  max=5s</t>
+  </si>
+  <si>
+    <t>T: 6t(63%): min = 5s,  max=30s;   RH(90%): 8s</t>
+  </si>
+  <si>
+    <t>https://srcsl.com/catalogoPDFs/SensoresProce/SensoresHumedad/MTH100.pdf</t>
   </si>
 </sst>
 </file>
@@ -1101,6 +1119,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1108,51 +1171,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3245,10 +3263,10 @@
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3299,10 +3317,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3353,10 +3371,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3404,24 +3422,24 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="46"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="32" t="s">
@@ -3449,10 +3467,10 @@
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="40"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3500,7 +3518,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="42" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3509,123 +3527,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="36" t="s">
+      <c r="Q9" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="48">
         <v>90</v>
       </c>
-      <c r="S9" s="36" t="s">
+      <c r="S9" s="42" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="37"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="37"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="43"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="37"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="37"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="43"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="38"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="38"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="44"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -3790,22 +3808,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3813,6 +3815,22 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3824,8 +3842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418314EB-8B6F-4509-AC06-8A64A9DA32C2}">
   <dimension ref="B2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3834,11 +3852,12 @@
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" customWidth="1"/>
     <col min="13" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="78.140625" customWidth="1"/>
   </cols>
@@ -3995,7 +4014,7 @@
     </row>
     <row r="6" spans="2:15" ht="45">
       <c r="B6" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>198</v>
@@ -4025,37 +4044,61 @@
         <v>214</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="45">
       <c r="B7" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="N7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="O7" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>226</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se crea la hoja de sensores en el excel y se agrega el primer sensor de ph.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F695A8-7EDB-4680-A90C-3F37305BDD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B57863C-E5E6-4070-93B3-F4A57139D077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="4740" windowWidth="9405" windowHeight="11520" firstSheet="2" activeTab="2" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="10905" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="3" activeTab="3" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
     <sheet name="Sensores temperatura automat" sheetId="2" r:id="rId2"/>
     <sheet name="Sensores de humedad" sheetId="3" r:id="rId3"/>
+    <sheet name="sensores de ph" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="242">
   <si>
     <t>Nombre</t>
   </si>
@@ -805,6 +806,51 @@
   </si>
   <si>
     <t>https://srcsl.com/catalogoPDFs/SensoresProce/SensoresHumedad/MTH100.pdf</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Tamperatura de medición</t>
+  </si>
+  <si>
+    <t>Tiempo de respuesta</t>
+  </si>
+  <si>
+    <t>Tamaño del módulo</t>
+  </si>
+  <si>
+    <t>Tipo de conector del sensor</t>
+  </si>
+  <si>
+    <t>SENSOR DE PH ANALÓGICO PARA ARDUINO</t>
+  </si>
+  <si>
+    <t>DFROBOT ITEM #SEN0161</t>
+  </si>
+  <si>
+    <t>5 VDC</t>
+  </si>
+  <si>
+    <t>0 -14 PH</t>
+  </si>
+  <si>
+    <t>0 - 60°C</t>
+  </si>
+  <si>
+    <t>(25°C) +/- 0.1 pH</t>
+  </si>
+  <si>
+    <t>&gt;= 1 min</t>
+  </si>
+  <si>
+    <t>43 * 32 mm</t>
+  </si>
+  <si>
+    <t>Conector BNC</t>
+  </si>
+  <si>
+    <t>https://www.vistronica.com/sensores/sensor-de-ph-analogico-para-arduino-detail.html</t>
   </si>
 </sst>
 </file>
@@ -889,7 +935,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,6 +963,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1023,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1119,6 +1171,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1140,41 +1225,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1185,6 +1240,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FFCC"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FF66FFCC"/>
@@ -3263,10 +3319,10 @@
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3317,10 +3373,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3371,10 +3427,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3422,24 +3478,24 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="35"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="46"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="32" t="s">
@@ -3467,10 +3523,10 @@
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3518,7 +3574,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="36" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3527,123 +3583,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="48">
+      <c r="R9" s="33">
         <v>90</v>
       </c>
-      <c r="S9" s="42" t="s">
+      <c r="S9" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="43"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="43"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="37"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="43"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="43"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="37"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="44"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="44"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="38"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -3808,6 +3864,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3815,22 +3887,6 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3842,7 +3898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418314EB-8B6F-4509-AC06-8A64A9DA32C2}">
   <dimension ref="B2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4110,4 +4166,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5F0A7-1AE6-4C73-8CB3-36281CC6BCEF}">
+  <dimension ref="B3:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="53.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="30">
+      <c r="B3" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>231</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="60">
+      <c r="B4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="K4" s="23">
+        <v>148740</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se cagrega un segundo sensor de ph.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B57863C-E5E6-4070-93B3-F4A57139D077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E00542-EE96-4022-9FFE-86C9D9331A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10905" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="3" activeTab="3" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="255">
   <si>
     <t>Nombre</t>
   </si>
@@ -851,6 +851,45 @@
   </si>
   <si>
     <t>https://www.vistronica.com/sensores/sensor-de-ph-analogico-para-arduino-detail.html</t>
+  </si>
+  <si>
+    <t>Sensor analógico de pH (Básico)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alimentación </t>
+  </si>
+  <si>
+    <t>5 V</t>
+  </si>
+  <si>
+    <t>Temperatura de medición</t>
+  </si>
+  <si>
+    <t>0 - 14 pH</t>
+  </si>
+  <si>
+    <t>0 - 80°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonda de pH </t>
+  </si>
+  <si>
+    <t>con conector BNC</t>
+  </si>
+  <si>
+    <t>Controlador pH 2.0</t>
+  </si>
+  <si>
+    <t>3 pines</t>
+  </si>
+  <si>
+    <t>Indicador LED</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>https://tienda.bricogeek.com/home/581-sensor-analogico-de-ph.html</t>
   </si>
 </sst>
 </file>
@@ -1168,9 +1207,57 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1180,56 +1267,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2915,25 +2954,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="13" t="s">
@@ -3294,35 +3333,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
     </row>
     <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3373,10 +3412,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3427,10 +3466,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3478,55 +3517,55 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="46"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
     </row>
     <row r="8" spans="2:19" ht="69" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="40"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3574,7 +3613,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="43" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3583,123 +3622,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="36" t="s">
+      <c r="Q9" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="49">
         <v>90</v>
       </c>
-      <c r="S9" s="36" t="s">
+      <c r="S9" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="37"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="37"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="44"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="37"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="37"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="44"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="38"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="38"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="45"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -3864,22 +3903,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3887,6 +3910,22 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3919,22 +3958,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
     </row>
     <row r="3" spans="2:15" ht="60">
       <c r="B3" s="31" t="s">
@@ -4170,59 +4209,61 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5F0A7-1AE6-4C73-8CB3-36281CC6BCEF}">
-  <dimension ref="B3:L4"/>
+  <dimension ref="B3:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="30">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="60">
+    <row r="4" spans="2:12" ht="45">
       <c r="B4" s="1" t="s">
         <v>232</v>
       </c>
@@ -4255,6 +4296,76 @@
       </c>
       <c r="L4" s="1" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="30">
+      <c r="B5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="30">
+      <c r="B6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crea una hoja de mdot lora vs esp32 y se agrega la tabla.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E00542-EE96-4022-9FFE-86C9D9331A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17856B-2A04-4A55-93D3-8060A6B88CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="3" activeTab="3" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
+    <workbookView xWindow="10905" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="4" activeTab="4" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensores de temperatura" sheetId="1" r:id="rId1"/>
     <sheet name="Sensores temperatura automat" sheetId="2" r:id="rId2"/>
     <sheet name="Sensores de humedad" sheetId="3" r:id="rId3"/>
     <sheet name="sensores de ph" sheetId="4" r:id="rId4"/>
+    <sheet name="mdotLORA vs ESP32" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="315">
   <si>
     <t>Nombre</t>
   </si>
@@ -891,6 +892,205 @@
   <si>
     <t>https://tienda.bricogeek.com/home/581-sensor-analogico-de-ph.html</t>
   </si>
+  <si>
+    <t>MultiTech mDot™   Long Range LoRa® Modules
+(MTDOT Series)</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>STMicroelectronics STM32F411RET</t>
+  </si>
+  <si>
+    <t>Max Clock</t>
+  </si>
+  <si>
+    <t>100MHz</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>512KB Flash (400KB customer usable)</t>
+  </si>
+  <si>
+    <t>128KB RAM</t>
+  </si>
+  <si>
+    <t>Radio Frequency</t>
+  </si>
+  <si>
+    <t>860MHz to 1020MHz</t>
+  </si>
+  <si>
+    <t>FSK, GFSK, MSK, GMSK, OOK, LoRa Digital Spread Spectrum</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>MTDOT-868: Europe</t>
+  </si>
+  <si>
+    <t>MTDOT-915: North America and Australia</t>
+  </si>
+  <si>
+    <t>MTDOT-923: Asia and Pacific</t>
+  </si>
+  <si>
+    <t>Comunication</t>
+  </si>
+  <si>
+    <t>LoRaWAN 1.0.2 compliant, Class A and Class C</t>
+  </si>
+  <si>
+    <t>Arm Mbed libraries or AT commands for radio control</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Up to 21 Digital I/O</t>
+  </si>
+  <si>
+    <t>Up to 11 Analog Inputs</t>
+  </si>
+  <si>
+    <t>Pin functions are multiplexed</t>
+  </si>
+  <si>
+    <t>Maximum transmitter power output</t>
+  </si>
+  <si>
+    <t>MTDOT-868: 14dBm</t>
+  </si>
+  <si>
+    <t>MTDOT-915: 19dBm</t>
+  </si>
+  <si>
+    <t>MTDOT-923: Varies by country</t>
+  </si>
+  <si>
+    <t>Maximum receive sensitivity</t>
+  </si>
+  <si>
+    <t>MTDOT-868: -137dBm</t>
+  </si>
+  <si>
+    <t>MTDOT-915: -130dBm</t>
+  </si>
+  <si>
+    <t>Link budget</t>
+  </si>
+  <si>
+    <t>MTDOT-868: 151dB Point-to-Multipoint, 147dB Point-to-Point</t>
+  </si>
+  <si>
+    <t>MTDOT-915: 145dB Point-to-Multipoint, 147dB Point-to-Point</t>
+  </si>
+  <si>
+    <r>
+      <t>SPI, I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C, UART (RX, TX, RTS, CTS)</t>
+    </r>
+  </si>
+  <si>
+    <t>Maximum effective isotropic radiated power (EiRP)</t>
+  </si>
+  <si>
+    <t>MTDOT-868: 10dBm</t>
+  </si>
+  <si>
+    <t>MTDOT-915: 36dBm</t>
+  </si>
+  <si>
+    <t>Input voltage</t>
+  </si>
+  <si>
+    <t>3.3 V yo 5VDC +/- 5%</t>
+  </si>
+  <si>
+    <t>Operating Temperature</t>
+  </si>
+  <si>
+    <t>desde -40°C to 85°C</t>
+  </si>
+  <si>
+    <t>Storege Temperature</t>
+  </si>
+  <si>
+    <t>Relative humidity</t>
+  </si>
+  <si>
+    <t>20% to 90% RH non-condensing</t>
+  </si>
+  <si>
+    <t>physical Dimensions</t>
+  </si>
+  <si>
+    <t>25.5 mm * 37.3 mm</t>
+  </si>
+  <si>
+    <t>EMC Compliance</t>
+  </si>
+  <si>
+    <t>US: FCC Part 15 Class B</t>
+  </si>
+  <si>
+    <t>EU: EN 55022 Class B, EN 55024.</t>
+  </si>
+  <si>
+    <t>Canada: ICES-003</t>
+  </si>
+  <si>
+    <t>Radio Compilance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FCC 15.247, IC RSS-210, EU EN 300 220</t>
+  </si>
+  <si>
+    <t>Safety Compilance</t>
+  </si>
+  <si>
+    <t>UL/cUL 60950-1 2nd Ed., cUL 60950-1 2nd Ed., IEC 60950-1 2nd Ed., AS/NZS 60950.1</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>MIL-STD-810G: High Temp, Low Temp, Random Vibration</t>
+  </si>
+  <si>
+    <t>SAE J1455: Transit Drop and Handling Drop, Random Vibration, Swept-Sine Vibration</t>
+  </si>
+  <si>
+    <t>IEC68-2-1: Cold Temp.</t>
+  </si>
+  <si>
+    <t>IEC68-2-2: Dry Hea</t>
+  </si>
+  <si>
+    <t>ESP32</t>
+  </si>
+  <si>
+    <t>mdot LORA vs ESP32</t>
+  </si>
 </sst>
 </file>
 
@@ -902,7 +1102,7 @@
     <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,8 +1173,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,6 +1237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +1349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1213,6 +1448,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1234,41 +1502,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1279,6 +1567,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC99"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFFCCCC"/>
@@ -3358,10 +3647,10 @@
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3412,10 +3701,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3466,10 +3755,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3517,24 +3806,24 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="47"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="33" t="s">
@@ -3562,10 +3851,10 @@
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3613,7 +3902,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="37" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3622,123 +3911,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="43" t="s">
+      <c r="P9" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="43" t="s">
+      <c r="Q9" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="49">
+      <c r="R9" s="34">
         <v>90</v>
       </c>
-      <c r="S9" s="43" t="s">
+      <c r="S9" s="37" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="44"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="44"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="38"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="44"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="44"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="38"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="45"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="45"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="39"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -3903,6 +4192,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -3910,22 +4215,6 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4211,7 +4500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5F0A7-1AE6-4C73-8CB3-36281CC6BCEF}">
   <dimension ref="B3:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -4372,4 +4661,351 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4956B15-7A1C-4017-9B28-E28DE116A1E8}">
+  <dimension ref="A2:V9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="16" customWidth="1"/>
+    <col min="22" max="22" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" ht="28.5">
+      <c r="A2" s="53"/>
+      <c r="B2" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="71"/>
+    </row>
+    <row r="3" spans="1:22" ht="45">
+      <c r="A3" s="53"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>263</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>277</v>
+      </c>
+      <c r="K3" s="60" t="s">
+        <v>281</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="M3" s="60" t="s">
+        <v>288</v>
+      </c>
+      <c r="N3" s="60" t="s">
+        <v>291</v>
+      </c>
+      <c r="O3" s="60" t="s">
+        <v>293</v>
+      </c>
+      <c r="P3" s="60" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q3" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="R3" s="60" t="s">
+        <v>298</v>
+      </c>
+      <c r="S3" s="59" t="s">
+        <v>300</v>
+      </c>
+      <c r="T3" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="U3" s="60" t="s">
+        <v>306</v>
+      </c>
+      <c r="V3" s="59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="63.75" customHeight="1">
+      <c r="A4" s="53"/>
+      <c r="B4" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>261</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>264</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>267</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="I4" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="J4" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="K4" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="L4" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="M4" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="N4" s="66" t="s">
+        <v>292</v>
+      </c>
+      <c r="O4" s="66" t="s">
+        <v>294</v>
+      </c>
+      <c r="P4" s="66" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q4" s="66" t="s">
+        <v>297</v>
+      </c>
+      <c r="R4" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>301</v>
+      </c>
+      <c r="T4" s="66" t="s">
+        <v>305</v>
+      </c>
+      <c r="U4" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="V4" s="55" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="83.25" customHeight="1">
+      <c r="B5" s="61"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="64" t="s">
+        <v>268</v>
+      </c>
+      <c r="H5" s="65"/>
+      <c r="I5" s="64" t="s">
+        <v>275</v>
+      </c>
+      <c r="J5" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="K5" s="64" t="s">
+        <v>283</v>
+      </c>
+      <c r="L5" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="M5" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="64" t="s">
+        <v>302</v>
+      </c>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="55" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="51" customHeight="1">
+      <c r="B6" s="61"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>269</v>
+      </c>
+      <c r="H6" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="I6" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="J6" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="K6" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="L6" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="M6" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="64" t="s">
+        <v>303</v>
+      </c>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="25.5">
+      <c r="B7" s="61"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="64" t="s">
+        <v>276</v>
+      </c>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="55" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="B9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="U4:U7"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" tooltip="STMicroelectronics STM32F411RET Arm Cortex-M4 MCU" display="https://co.mouser.com/Semiconductors/Embedded-Processors-Controllers/Microcontrollers-MCU/ARM-Microcontrollers-MCU/STM32F411RE-Series/_/N-a85pc?P=1y8udoh&amp;Keyword=121374776&amp;FS=True&amp;Ntk=P_MarCom" xr:uid="{A68E4F11-5046-4C68-A336-C0E2AB8E3B94}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrrga información del ESP32 a la tabla.
</commit_message>
<xml_diff>
--- a/Documentos/comparativa_IOT.csv.xlsx
+++ b/Documentos/comparativa_IOT.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\proyectoIOT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17856B-2A04-4A55-93D3-8060A6B88CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D83729-1AF9-448E-8392-ACEF177C7C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10905" yWindow="0" windowWidth="9405" windowHeight="11520" firstSheet="4" activeTab="4" xr2:uid="{7E01FEB3-58F6-4820-BDCE-82585D8DC7F2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="354">
   <si>
     <t>Nombre</t>
   </si>
@@ -1091,6 +1091,123 @@
   <si>
     <t>mdot LORA vs ESP32</t>
   </si>
+  <si>
+    <t> microprocesador de 32-bit Xtensa LX6 de doble núcleo (o de un solo núcleo), operando a 160 o 240 MHz y rindiendo hasta 600 DMIPS</t>
+  </si>
+  <si>
+    <t>520 KiB SRAM</t>
+  </si>
+  <si>
+    <t>Procesador</t>
+  </si>
+  <si>
+    <t>ULP</t>
+  </si>
+  <si>
+    <t>Co-procesador de ultra baja energía</t>
+  </si>
+  <si>
+    <t>Memoria</t>
+  </si>
+  <si>
+    <t>Conectividad Inalambrica</t>
+  </si>
+  <si>
+    <t>802.11 b/g/n</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>Wi-Fi</t>
+  </si>
+  <si>
+    <t>v4.2 BR/EDR y BLE</t>
+  </si>
+  <si>
+    <t>Interfaces perifericas</t>
+  </si>
+  <si>
+    <t>12-bit SAR ADC de hasta 18 canales</t>
+  </si>
+  <si>
+    <t>2 × 8-bit DACs</t>
+  </si>
+  <si>
+    <t>10 × sensores de tacto (sensores capacitivos GPIOs)</t>
+  </si>
+  <si>
+    <t>4 × SPI</t>
+  </si>
+  <si>
+    <t>2 × interfaces I²S</t>
+  </si>
+  <si>
+    <t>2 × interfaces I²C</t>
+  </si>
+  <si>
+    <t>3 × UART</t>
+  </si>
+  <si>
+    <t>Controlador host SD/SDIO/CE-ATA/MMC/eMMC</t>
+  </si>
+  <si>
+    <t>Controlador esclavo SDIO/SPI</t>
+  </si>
+  <si>
+    <t>Bus CAN 2.0</t>
+  </si>
+  <si>
+    <t>Controlador remoto infrarrojo (TX/RX, hasta 8 canales)</t>
+  </si>
+  <si>
+    <t>Motor PWM</t>
+  </si>
+  <si>
+    <t>LED PWM (hasta 16 canales)</t>
+  </si>
+  <si>
+    <t>Sensor de efecto Hall</t>
+  </si>
+  <si>
+    <t>Pre-amplificador analógico de ultra baja potencia</t>
+  </si>
+  <si>
+    <t>Interfaz Ethernet MAC con DMA dedicado y soporte para el protocolo IEEE 1588 Precision Time Protocol</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Soporta todas las características de seguridad estándar de IEEE 802.11, incluyendo WFA, WPA/WPA2 y WAPI</t>
+  </si>
+  <si>
+    <t>Arranque seguro</t>
+  </si>
+  <si>
+    <t>Cifrado flash</t>
+  </si>
+  <si>
+    <t>1024-bit OTP, hasta 768-bit para clientes</t>
+  </si>
+  <si>
+    <t>Criptografía acelerada por hardware: AES, SHA-2, RSA, criptografía de curva elíptica (ECC), generador de números aleatorios (RNG)</t>
+  </si>
+  <si>
+    <t>Administración de energía</t>
+  </si>
+  <si>
+    <t>Regulador interno de baja caída</t>
+  </si>
+  <si>
+    <t>Dominio de poder individual para RTC</t>
+  </si>
+  <si>
+    <t>Corriente de 5μA en modo de suspensión profundo</t>
+  </si>
+  <si>
+    <t>Despierta por interrupción de GPIO, temporizador, medidas de ADC, interrupción por sensor de tacto capacitivo</t>
+  </si>
 </sst>
 </file>
 
@@ -1102,7 +1219,7 @@
     <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1201,6 +1318,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1349,7 +1477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1445,71 +1573,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1528,35 +1593,161 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1567,10 +1758,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFFFCC99"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFFCCCC"/>
       <color rgb="FF66FFCC"/>
     </mruColors>
   </colors>
@@ -3243,25 +3434,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:19" ht="60.75" customHeight="1">
       <c r="B3" s="13" t="s">
@@ -3622,35 +3813,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
     </row>
     <row r="3" spans="2:19" ht="60" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="13" t="s">
         <v>80</v>
       </c>
@@ -3701,10 +3892,10 @@
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="8" t="s">
         <v>79</v>
       </c>
@@ -3755,10 +3946,10 @@
       <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3806,55 +3997,55 @@
       </c>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="47"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="45"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
     </row>
     <row r="8" spans="2:19" ht="69" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="18" t="s">
         <v>121</v>
       </c>
@@ -3902,7 +4093,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="45" customHeight="1">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="52" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3911,123 +4102,123 @@
       <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="O9" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="P9" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="37" t="s">
+      <c r="Q9" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="R9" s="34">
+      <c r="R9" s="58">
         <v>90</v>
       </c>
-      <c r="S9" s="37" t="s">
+      <c r="S9" s="52" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="38"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="38"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="53"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="38"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="38"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="53"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="39"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="39"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="54"/>
     </row>
     <row r="13" spans="2:19" ht="30">
       <c r="B13" s="19"/>
@@ -4192,22 +4383,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B7:S7"/>
-    <mergeCell ref="B6:S6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L9:L12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="S9:S12"/>
     <mergeCell ref="M9:M12"/>
@@ -4215,6 +4390,22 @@
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B7:S7"/>
+    <mergeCell ref="B6:S6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4247,22 +4438,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="2:15" ht="60">
       <c r="B3" s="31" t="s">
@@ -4665,18 +4856,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4956B15-7A1C-4017-9B28-E28DE116A1E8}">
-  <dimension ref="A2:V9"/>
+  <dimension ref="A2:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+    <sheetView tabSelected="1" topLeftCell="L3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
@@ -4693,297 +4885,645 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" ht="28.5">
-      <c r="A2" s="53"/>
-      <c r="B2" s="69" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="71"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="67"/>
     </row>
     <row r="3" spans="1:22" ht="45">
-      <c r="A3" s="53"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="59" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="38" t="s">
         <v>266</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="L3" s="59" t="s">
+      <c r="L3" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="39" t="s">
         <v>288</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="39" t="s">
         <v>291</v>
       </c>
-      <c r="O3" s="60" t="s">
+      <c r="O3" s="39" t="s">
         <v>293</v>
       </c>
-      <c r="P3" s="60" t="s">
+      <c r="P3" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="Q3" s="60" t="s">
+      <c r="Q3" s="39" t="s">
         <v>296</v>
       </c>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="59" t="s">
+      <c r="S3" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="T3" s="60" t="s">
+      <c r="T3" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="U3" s="60" t="s">
+      <c r="U3" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="V3" s="59" t="s">
+      <c r="V3" s="38" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="63.75" customHeight="1">
-      <c r="A4" s="53"/>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="71" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="72" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="68" t="s">
         <v>261</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="68" t="s">
         <v>264</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="41" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="63" t="s">
+      <c r="H4" s="68" t="s">
         <v>271</v>
       </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="41" t="s">
         <v>274</v>
       </c>
-      <c r="J4" s="64" t="s">
+      <c r="J4" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="K4" s="64" t="s">
+      <c r="K4" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="L4" s="64" t="s">
+      <c r="L4" s="41" t="s">
         <v>285</v>
       </c>
-      <c r="M4" s="64" t="s">
+      <c r="M4" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="70" t="s">
         <v>292</v>
       </c>
-      <c r="O4" s="66" t="s">
+      <c r="O4" s="70" t="s">
         <v>294</v>
       </c>
-      <c r="P4" s="66" t="s">
+      <c r="P4" s="70" t="s">
         <v>294</v>
       </c>
-      <c r="Q4" s="66" t="s">
+      <c r="Q4" s="70" t="s">
         <v>297</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="70" t="s">
         <v>299</v>
       </c>
-      <c r="S4" s="64" t="s">
+      <c r="S4" s="41" t="s">
         <v>301</v>
       </c>
-      <c r="T4" s="66" t="s">
+      <c r="T4" s="70" t="s">
         <v>305</v>
       </c>
-      <c r="U4" s="66" t="s">
+      <c r="U4" s="70" t="s">
         <v>307</v>
       </c>
-      <c r="V4" s="55" t="s">
+      <c r="V4" s="34" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="83.25" customHeight="1">
-      <c r="B5" s="61"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="64" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="64" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="K5" s="64" t="s">
+      <c r="K5" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="M5" s="64" t="s">
+      <c r="M5" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="64" t="s">
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="41" t="s">
         <v>302</v>
       </c>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="55" t="s">
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="34" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1">
-      <c r="B6" s="61"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63" t="s">
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="68" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="63" t="s">
+      <c r="F6" s="68" t="s">
         <v>265</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="68" t="s">
         <v>272</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="J6" s="64" t="s">
+      <c r="J6" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="K6" s="64" t="s">
+      <c r="K6" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="L6" s="64" t="s">
+      <c r="L6" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="64" t="s">
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="55" t="s">
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="34" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="25.5">
-      <c r="B7" s="61"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="64" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
-      <c r="V7" s="55" t="s">
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="34" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
+    <row r="8" spans="1:22" ht="33.75" customHeight="1">
+      <c r="B8" s="37"/>
+      <c r="C8" s="73" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="74" t="s">
+        <v>320</v>
+      </c>
+      <c r="F8" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="G8" s="77"/>
+      <c r="H8" s="74" t="s">
+        <v>326</v>
+      </c>
+      <c r="I8" s="75" t="s">
+        <v>343</v>
+      </c>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75" t="s">
+        <v>349</v>
+      </c>
+      <c r="M8" s="75"/>
+      <c r="N8" s="92"/>
+      <c r="O8" s="92"/>
+      <c r="P8" s="92"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
     </row>
-    <row r="9" spans="1:22">
-      <c r="B9" t="s">
+    <row r="9" spans="1:22" ht="105" customHeight="1">
+      <c r="B9" s="85" t="s">
         <v>313</v>
       </c>
+      <c r="C9" s="80" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="80" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>324</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>327</v>
+      </c>
+      <c r="I9" s="80" t="s">
+        <v>344</v>
+      </c>
+      <c r="J9" s="86" t="s">
+        <v>346</v>
+      </c>
+      <c r="K9" s="86" t="s">
+        <v>348</v>
+      </c>
+      <c r="L9" s="80" t="s">
+        <v>350</v>
+      </c>
+      <c r="M9" s="80" t="s">
+        <v>352</v>
+      </c>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="B10" s="85"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="40" t="s">
+        <v>328</v>
+      </c>
+      <c r="I10" s="80"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+    </row>
+    <row r="11" spans="1:22" ht="30">
+      <c r="B11" s="85"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="78" t="s">
+        <v>329</v>
+      </c>
+      <c r="I11" s="80"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="B12" s="85"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="78" t="s">
+        <v>330</v>
+      </c>
+      <c r="I12" s="80"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="B13" s="85"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="78" t="s">
+        <v>331</v>
+      </c>
+      <c r="I13" s="80"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="B14" s="85"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="78" t="s">
+        <v>332</v>
+      </c>
+      <c r="I14" s="80"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="B15" s="85"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="78" t="s">
+        <v>333</v>
+      </c>
+      <c r="I15" s="80"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+    </row>
+    <row r="16" spans="1:22" ht="42.75" customHeight="1">
+      <c r="B16" s="85"/>
+      <c r="C16" s="84" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16" s="81" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16" s="80"/>
+      <c r="F16" s="62" t="s">
+        <v>323</v>
+      </c>
+      <c r="G16" s="79" t="s">
+        <v>325</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>334</v>
+      </c>
+      <c r="I16" s="84" t="s">
+        <v>345</v>
+      </c>
+      <c r="J16" s="52" t="s">
+        <v>347</v>
+      </c>
+      <c r="K16" s="87"/>
+      <c r="L16" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="M16" s="84" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="85"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="78" t="s">
+        <v>335</v>
+      </c>
+      <c r="I17" s="84"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="84"/>
+    </row>
+    <row r="18" spans="2:13" ht="60">
+      <c r="B18" s="85"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="78" t="s">
+        <v>342</v>
+      </c>
+      <c r="I18" s="84"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="84"/>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="85"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="I19" s="84"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+    </row>
+    <row r="20" spans="2:13" ht="30">
+      <c r="B20" s="85"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="78" t="s">
+        <v>337</v>
+      </c>
+      <c r="I20" s="84"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="85"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="78" t="s">
+        <v>338</v>
+      </c>
+      <c r="I21" s="84"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="85"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="78" t="s">
+        <v>339</v>
+      </c>
+      <c r="I22" s="84"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="85"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="78" t="s">
+        <v>340</v>
+      </c>
+      <c r="I23" s="84"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
+    </row>
+    <row r="24" spans="2:13" ht="30">
+      <c r="B24" s="85"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="78" t="s">
+        <v>341</v>
+      </c>
+      <c r="I24" s="84"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="40">
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="K9:K24"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:L15"/>
+    <mergeCell ref="L16:L24"/>
+    <mergeCell ref="M9:M15"/>
+    <mergeCell ref="M16:M24"/>
+    <mergeCell ref="B9:B24"/>
+    <mergeCell ref="C16:C24"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="I16:I24"/>
+    <mergeCell ref="J9:J15"/>
+    <mergeCell ref="J16:J24"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="G16:G24"/>
+    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="E9:E24"/>
+    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="D16:D24"/>
+    <mergeCell ref="C9:C15"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="B2:V2"/>
     <mergeCell ref="N4:N7"/>
@@ -5000,7 +5540,6 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" tooltip="STMicroelectronics STM32F411RET Arm Cortex-M4 MCU" display="https://co.mouser.com/Semiconductors/Embedded-Processors-Controllers/Microcontrollers-MCU/ARM-Microcontrollers-MCU/STM32F411RE-Series/_/N-a85pc?P=1y8udoh&amp;Keyword=121374776&amp;FS=True&amp;Ntk=P_MarCom" xr:uid="{A68E4F11-5046-4C68-A336-C0E2AB8E3B94}"/>

</xml_diff>